<commit_message>
nabin sir quantity calculaed, kar samayojan, naksha faram bhareko
</commit_message>
<xml_diff>
--- a/ofc/estimates/ganapati baatika mandir samrakxan/valuation ganapati batika pahiro samrakxan.xlsx
+++ b/ofc/estimates/ganapati baatika mandir samrakxan/valuation ganapati batika pahiro samrakxan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="re-estimate" sheetId="18" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="description_781">[6]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'re-estimate'!$A$1:$K$39</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'re-estimate'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
@@ -534,24 +534,6 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -562,6 +544,39 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -578,21 +593,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1322,113 +1322,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="A2" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -1991,11 +1991,11 @@
       <c r="B34" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="67">
+      <c r="C34" s="61">
         <f>J32</f>
         <v>568746.79695333343</v>
       </c>
-      <c r="D34" s="67"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="38">
         <v>100</v>
       </c>
@@ -2011,10 +2011,10 @@
       <c r="B35" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="70">
+      <c r="C35" s="64">
         <v>500000</v>
       </c>
-      <c r="D35" s="70"/>
+      <c r="D35" s="64"/>
       <c r="E35" s="38"/>
       <c r="F35" s="44"/>
       <c r="G35" s="43"/>
@@ -2028,11 +2028,11 @@
       <c r="B36" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="70">
+      <c r="C36" s="64">
         <f>C35-C38-C39</f>
         <v>475000</v>
       </c>
-      <c r="D36" s="70"/>
+      <c r="D36" s="64"/>
       <c r="E36" s="38">
         <f>C36/C34*100</f>
         <v>83.516953861451725</v>
@@ -2049,11 +2049,11 @@
       <c r="B37" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="67">
+      <c r="C37" s="61">
         <f>C34-C36</f>
         <v>93746.796953333425</v>
       </c>
-      <c r="D37" s="67"/>
+      <c r="D37" s="61"/>
       <c r="E37" s="38">
         <f>100-E36</f>
         <v>16.483046138548275</v>
@@ -2070,11 +2070,11 @@
       <c r="B38" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="67">
+      <c r="C38" s="61">
         <f>C35*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D38" s="67"/>
+      <c r="D38" s="61"/>
       <c r="E38" s="38">
         <v>3</v>
       </c>
@@ -2090,11 +2090,11 @@
       <c r="B39" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="67">
+      <c r="C39" s="61">
         <f>C35*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D39" s="67"/>
+      <c r="D39" s="61"/>
       <c r="E39" s="38">
         <v>2</v>
       </c>
@@ -2176,6 +2176,13 @@
     <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="A7:F7"/>
@@ -2184,13 +2191,6 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2210,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2230,90 +2230,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
+      <c r="A2" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="77">
+      <c r="C6" s="71">
         <f>F26</f>
         <v>568746.79695333343</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="72"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2321,11 +2321,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="77">
+      <c r="J6" s="71">
         <f>I26</f>
-        <v>518004.34040666668</v>
-      </c>
-      <c r="K6" s="78"/>
+        <v>568854.64608666673</v>
+      </c>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
@@ -2334,77 +2334,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="I7" s="74" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="61" t="str">
+      <c r="A8" s="65" t="str">
         <f>'re-estimate'!A6:F6</f>
         <v>Project:- गणपती गणेश मन्दिर मनोहरा नदीबाट कटान संरक्षण गर्ने</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="I8" s="75" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="I8" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="61" t="str">
+      <c r="A9" s="65" t="str">
         <f>'re-estimate'!A7:F7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="I9" s="75" t="s">
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="I9" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76" t="s">
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="71" t="s">
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="72" t="s">
+      <c r="K11" s="77" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2423,8 +2423,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="72"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="77"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
@@ -2452,20 +2452,20 @@
         <v>2436.5509999999999</v>
       </c>
       <c r="G13" s="12">
-        <f>V!G11</f>
-        <v>40.600000000000009</v>
+        <f>V!G12</f>
+        <v>45.099999999999994</v>
       </c>
       <c r="H13" s="12">
-        <f>V!I11</f>
+        <f>V!I12</f>
         <v>64.63</v>
       </c>
       <c r="I13" s="12">
         <f>G13*H13</f>
-        <v>2623.9780000000005</v>
+        <v>2914.8129999999996</v>
       </c>
       <c r="J13" s="27">
         <f>I13-F13</f>
-        <v>187.42700000000059</v>
+        <v>478.26199999999972</v>
       </c>
       <c r="K13" s="14"/>
     </row>
@@ -2485,12 +2485,12 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12">
-        <f>V!J12</f>
-        <v>282.72486666666674</v>
+        <f>V!J13</f>
+        <v>314.06136666666663</v>
       </c>
       <c r="J14" s="27">
         <f>I14-F14</f>
-        <v>20.194633333333343</v>
+        <v>51.53113333333323</v>
       </c>
       <c r="K14" s="14"/>
     </row>
@@ -2533,20 +2533,20 @@
         <v>2627.8199999999997</v>
       </c>
       <c r="G16" s="12">
-        <f>V!G16</f>
-        <v>7</v>
+        <f>V!G18</f>
+        <v>6.8</v>
       </c>
       <c r="H16" s="12">
-        <f>V!I16</f>
+        <f>V!I18</f>
         <v>404.28</v>
       </c>
       <c r="I16" s="12">
         <f>G16*H16</f>
-        <v>2829.96</v>
+        <v>2749.1039999999998</v>
       </c>
       <c r="J16" s="27">
         <f>I16-F16</f>
-        <v>202.14000000000033</v>
+        <v>121.28400000000011</v>
       </c>
       <c r="K16" s="14"/>
     </row>
@@ -2589,20 +2589,20 @@
         <v>507725.4</v>
       </c>
       <c r="G18" s="12">
-        <f>V!G22</f>
-        <v>71</v>
+        <f>V!G24</f>
+        <v>78</v>
       </c>
       <c r="H18" s="12">
-        <f>V!I22</f>
+        <f>V!I24</f>
         <v>6509.3</v>
       </c>
       <c r="I18" s="12">
         <f>G18*H18</f>
-        <v>462160.3</v>
+        <v>507725.4</v>
       </c>
       <c r="J18" s="27">
         <f>I18-F18</f>
-        <v>-45565.100000000035</v>
+        <v>0</v>
       </c>
       <c r="K18" s="14"/>
     </row>
@@ -2622,12 +2622,12 @@
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12">
-        <f>V!J23</f>
-        <v>43812.945540000001</v>
+        <f>V!J25</f>
+        <v>48132.531719999999</v>
       </c>
       <c r="J19" s="27">
         <f>I19-F19</f>
-        <v>-4319.5861799999984</v>
+        <v>0</v>
       </c>
       <c r="K19" s="14"/>
     </row>
@@ -2670,20 +2670,20 @@
         <v>6295.3799999999992</v>
       </c>
       <c r="G21" s="12">
-        <f>V!G29</f>
-        <v>32</v>
+        <f>V!G32</f>
+        <v>36</v>
       </c>
       <c r="H21" s="12">
-        <f>V!I29</f>
+        <f>V!I32</f>
         <v>161.41999999999999</v>
       </c>
       <c r="I21" s="12">
         <f>G21*H21</f>
-        <v>5165.4399999999996</v>
+        <v>5811.12</v>
       </c>
       <c r="J21" s="27">
         <f>I21-F21</f>
-        <v>-1129.9399999999996</v>
+        <v>-484.25999999999931</v>
       </c>
       <c r="K21" s="14"/>
     </row>
@@ -2703,12 +2703,12 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12">
-        <f>V!J30</f>
-        <v>628.99200000000008</v>
+        <f>V!J33</f>
+        <v>707.61599999999999</v>
       </c>
       <c r="J22" s="27">
         <f>I22-F22</f>
-        <v>-137.59199999999998</v>
+        <v>-58.968000000000075</v>
       </c>
       <c r="K22" s="14"/>
     </row>
@@ -2751,11 +2751,11 @@
         <v>500</v>
       </c>
       <c r="G24" s="12">
-        <f>V!G32</f>
+        <f>V!G35</f>
         <v>1</v>
       </c>
       <c r="H24" s="12">
-        <f>V!I32</f>
+        <f>V!I35</f>
         <v>500</v>
       </c>
       <c r="I24" s="12">
@@ -2797,23 +2797,16 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7">
         <f>SUM(I13:I24)</f>
-        <v>518004.34040666668</v>
+        <v>568854.64608666673</v>
       </c>
       <c r="J26" s="13">
         <f>I26-F26</f>
-        <v>-50742.456546666741</v>
+        <v>107.84913333330769</v>
       </c>
       <c r="K26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2827,6 +2820,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2842,10 +2842,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N98"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2863,113 +2863,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
+      <c r="A2" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -3032,18 +3032,19 @@
         <v>1</v>
       </c>
       <c r="D10" s="37">
-        <v>14</v>
+        <f>13</f>
+        <v>13</v>
       </c>
       <c r="E10" s="37">
-        <f>2.5+0.2+0.2</f>
-        <v>2.9000000000000004</v>
+        <f>2.5+0.3+0.3</f>
+        <v>3.0999999999999996</v>
       </c>
       <c r="F10" s="37">
         <v>1</v>
       </c>
       <c r="G10" s="38">
         <f>PRODUCT(C10:F10)</f>
-        <v>40.600000000000009</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
@@ -3052,50 +3053,59 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
-      <c r="B11" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="23">
-        <f>SUM(G10:G10)</f>
-        <v>40.600000000000009</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="23">
-        <v>64.63</v>
-      </c>
-      <c r="J11" s="40">
-        <f>G11*I11</f>
-        <v>2623.9780000000005</v>
-      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="35">
+        <v>1</v>
+      </c>
+      <c r="D11" s="37">
+        <v>2</v>
+      </c>
+      <c r="E11" s="37">
+        <f>2+0.2+0.2</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="F11" s="37">
+        <v>1</v>
+      </c>
+      <c r="G11" s="38">
+        <f>PRODUCT(C11:F11)</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
       <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="36" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
+      <c r="G12" s="23">
+        <f>SUM(G10:G11)</f>
+        <v>45.099999999999994</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="23">
+        <v>64.63</v>
+      </c>
       <c r="J12" s="40">
-        <f>0.13*G11*19284/360</f>
-        <v>282.72486666666674</v>
-      </c>
-      <c r="K12" s="60"/>
+        <f>G12*I12</f>
+        <v>2914.8129999999996</v>
+      </c>
+      <c r="K12" s="58"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
-      <c r="B13" s="36"/>
+      <c r="B13" s="36" t="s">
+        <v>45</v>
+      </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -3103,16 +3113,15 @@
       <c r="G13" s="23"/>
       <c r="H13" s="22"/>
       <c r="I13" s="23"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="21"/>
-    </row>
-    <row r="14" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
-        <v>2</v>
-      </c>
-      <c r="B14" s="59" t="s">
-        <v>48</v>
-      </c>
+      <c r="J13" s="40">
+        <f>0.13*G12*19284/360</f>
+        <v>314.06136666666663</v>
+      </c>
+      <c r="K13" s="60"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -3123,29 +3132,18 @@
       <c r="J14" s="40"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="36" t="str">
-        <f>B10</f>
-        <v>-for gabion wall</v>
-      </c>
-      <c r="C15" s="19">
-        <v>1</v>
-      </c>
-      <c r="D15" s="20">
-        <v>14</v>
-      </c>
-      <c r="E15" s="21">
-        <f>0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="21">
-        <v>1</v>
-      </c>
-      <c r="G15" s="38">
-        <f>PRODUCT(C15:F15)</f>
-        <v>7</v>
-      </c>
+    <row r="15" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
       <c r="J15" s="40"/>
@@ -3153,119 +3151,121 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
-      <c r="B16" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="23">
-        <f>SUM(G15:G15)</f>
-        <v>7</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="23">
-        <v>404.28</v>
-      </c>
-      <c r="J16" s="40">
-        <f>G16*I16</f>
-        <v>2829.96</v>
-      </c>
+      <c r="B16" s="36" t="str">
+        <f>B10</f>
+        <v>-for gabion wall</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20">
+        <v>13</v>
+      </c>
+      <c r="E16" s="21">
+        <f>0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="21">
+        <v>1</v>
+      </c>
+      <c r="G16" s="38">
+        <f>PRODUCT(C16:F16)</f>
+        <v>6.5</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="40"/>
       <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="23"/>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="20">
+        <v>2</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="38">
+        <f>PRODUCT(C17:F17)</f>
+        <v>0.3</v>
+      </c>
       <c r="H17" s="22"/>
       <c r="I17" s="23"/>
       <c r="J17" s="40"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="193.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
-        <v>3</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>44</v>
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="36" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="60"/>
+      <c r="G18" s="23">
+        <f>SUM(G16:G17)</f>
+        <v>6.8</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="23">
+        <v>404.28</v>
+      </c>
+      <c r="J18" s="40">
+        <f>G18*I18</f>
+        <v>2749.1039999999998</v>
+      </c>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
-      <c r="B19" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="35">
-        <v>1</v>
-      </c>
-      <c r="D19" s="37">
+      <c r="B19" s="36"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="1:14" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
         <v>3</v>
       </c>
-      <c r="E19" s="37">
-        <v>1</v>
-      </c>
-      <c r="F19" s="37">
-        <v>1</v>
-      </c>
-      <c r="G19" s="38">
-        <f>PRODUCT(C19:F19)</f>
-        <v>3</v>
-      </c>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="58"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="35">
-        <f>(4+2+2)+8+3</f>
-        <v>19</v>
-      </c>
-      <c r="D20" s="37">
-        <v>2</v>
-      </c>
-      <c r="E20" s="37">
-        <v>1</v>
-      </c>
-      <c r="F20" s="37">
-        <v>1</v>
-      </c>
-      <c r="G20" s="38">
-        <f t="shared" ref="G20:G21" si="0">PRODUCT(C20:F20)</f>
-        <v>38</v>
-      </c>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="58"/>
+      <c r="B20" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="60"/>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
-      <c r="B21" s="36"/>
+      <c r="B21" s="36" t="s">
+        <v>43</v>
+      </c>
       <c r="C21" s="35">
-        <f>(8+4)+(2+4)+2</f>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D21" s="37">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E21" s="37">
         <v>1</v>
@@ -3274,8 +3274,8 @@
         <v>1</v>
       </c>
       <c r="G21" s="38">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f>PRODUCT(C21:F21)</f>
+        <v>3</v>
       </c>
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
@@ -3284,74 +3284,91 @@
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
-      <c r="B22" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="23">
-        <f>SUM(G19:G21)</f>
-        <v>71</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="23">
-        <v>6509.3</v>
-      </c>
-      <c r="J22" s="40">
-        <f>G22*I22</f>
-        <v>462160.3</v>
-      </c>
-      <c r="K22" s="21"/>
-      <c r="M22">
-        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
-        <v>7485.69</v>
-      </c>
-      <c r="N22">
-        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
-        <v>4746.7977499999997</v>
-      </c>
+      <c r="B22" s="36"/>
+      <c r="C22" s="35">
+        <f>(4+2+2)+8+3+2</f>
+        <v>21</v>
+      </c>
+      <c r="D22" s="37">
+        <v>2</v>
+      </c>
+      <c r="E22" s="37">
+        <v>1</v>
+      </c>
+      <c r="F22" s="37">
+        <v>1</v>
+      </c>
+      <c r="G22" s="38">
+        <f t="shared" ref="G22:G23" si="0">PRODUCT(C22:F22)</f>
+        <v>42</v>
+      </c>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="58"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
-      <c r="B23" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="40">
-        <f>0.13*G22*4746.798</f>
-        <v>43812.945540000001</v>
-      </c>
-      <c r="K23" s="21"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="35">
+        <f>(8+4)+(2+4)+2+2</f>
+        <v>22</v>
+      </c>
+      <c r="D23" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="E23" s="37">
+        <v>1</v>
+      </c>
+      <c r="F23" s="37">
+        <v>1</v>
+      </c>
+      <c r="G23" s="38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="58"/>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
-      <c r="B24" s="36"/>
+      <c r="B24" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="40"/>
+      <c r="G24" s="23">
+        <f>SUM(G21:G23)</f>
+        <v>78</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="23">
+        <v>6509.3</v>
+      </c>
+      <c r="J24" s="40">
+        <f>G24*I24</f>
+        <v>507725.4</v>
+      </c>
       <c r="K24" s="21"/>
-    </row>
-    <row r="25" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
-        <v>4</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>46</v>
+      <c r="M24">
+        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
+        <v>7485.69</v>
+      </c>
+      <c r="N24">
+        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
+        <v>4746.7977499999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="36" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
@@ -3360,71 +3377,60 @@
       <c r="G25" s="23"/>
       <c r="H25" s="22"/>
       <c r="I25" s="23"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="58"/>
+      <c r="J25" s="40">
+        <f>0.13*G24*4746.798</f>
+        <v>48132.531719999999</v>
+      </c>
+      <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
-      <c r="B26" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="35">
-        <v>1</v>
-      </c>
-      <c r="D26" s="37">
-        <v>14</v>
-      </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37">
-        <v>1</v>
-      </c>
-      <c r="G26" s="38">
-        <f>PRODUCT(C26:F26)</f>
-        <v>14</v>
-      </c>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="40"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="35">
-        <v>1</v>
-      </c>
-      <c r="D27" s="37">
-        <v>12</v>
-      </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37">
-        <v>1</v>
-      </c>
-      <c r="G27" s="38">
-        <f t="shared" ref="G27:G28" si="1">PRODUCT(C27:F27)</f>
-        <v>12</v>
-      </c>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="21"/>
+    <row r="27" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
+        <v>4</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="58"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
-      <c r="B28" s="36"/>
+      <c r="B28" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="C28" s="35">
         <v>1</v>
       </c>
       <c r="D28" s="37">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E28" s="37"/>
       <c r="F28" s="37">
         <v>1</v>
       </c>
       <c r="G28" s="38">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>PRODUCT(C28:F28)</f>
+        <v>14</v>
       </c>
       <c r="H28" s="39"/>
       <c r="I28" s="39"/>
@@ -3433,100 +3439,108 @@
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
-      <c r="B29" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="23">
-        <f>SUM(G26:G28)</f>
-        <v>32</v>
-      </c>
-      <c r="H29" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I29" s="23">
-        <v>161.41999999999999</v>
-      </c>
-      <c r="J29" s="40">
-        <f>G29*I29</f>
-        <v>5165.4399999999996</v>
-      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="35">
+        <v>1</v>
+      </c>
+      <c r="D29" s="37">
+        <v>12</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37">
+        <v>1</v>
+      </c>
+      <c r="G29" s="38">
+        <f t="shared" ref="G29:G31" si="1">PRODUCT(C29:F29)</f>
+        <v>12</v>
+      </c>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
       <c r="K29" s="21"/>
-      <c r="M29">
-        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
-        <v>7485.69</v>
-      </c>
-      <c r="N29">
-        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
-        <v>4746.7977499999997</v>
-      </c>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
-      <c r="B30" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="40">
-        <f>0.13*G29*45360/300</f>
-        <v>628.99200000000008</v>
-      </c>
+      <c r="B30" s="36"/>
+      <c r="C30" s="35">
+        <v>1</v>
+      </c>
+      <c r="D30" s="37">
+        <v>6</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37">
+        <v>1</v>
+      </c>
+      <c r="G30" s="38">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
       <c r="K30" s="21"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="36"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="40"/>
+      <c r="C31" s="35">
+        <v>1</v>
+      </c>
+      <c r="D31" s="37">
+        <v>2</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37">
+        <v>2</v>
+      </c>
+      <c r="G31" s="38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
       <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18">
-        <v>5</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="19">
-        <v>1</v>
-      </c>
+      <c r="A32" s="18"/>
+      <c r="B32" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
-      <c r="G32" s="33">
-        <f t="shared" ref="G32" si="2">PRODUCT(C32:F32)</f>
-        <v>1</v>
+      <c r="G32" s="23">
+        <f>SUM(G28:G31)</f>
+        <v>36</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="I32" s="23">
-        <v>500</v>
-      </c>
-      <c r="J32" s="33">
+        <v>161.41999999999999</v>
+      </c>
+      <c r="J32" s="40">
         <f>G32*I32</f>
-        <v>500</v>
+        <v>5811.12</v>
       </c>
       <c r="K32" s="21"/>
+      <c r="M32">
+        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
+        <v>7485.69</v>
+      </c>
+      <c r="N32">
+        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
+        <v>4746.7977499999997</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18"/>
-      <c r="B33" s="24"/>
+      <c r="B33" s="36" t="s">
+        <v>45</v>
+      </c>
       <c r="C33" s="19"/>
       <c r="D33" s="20"/>
       <c r="E33" s="21"/>
@@ -3534,132 +3548,128 @@
       <c r="G33" s="23"/>
       <c r="H33" s="22"/>
       <c r="I33" s="23"/>
-      <c r="J33" s="40"/>
+      <c r="J33" s="40">
+        <f>0.13*G32*45360/300</f>
+        <v>707.61599999999999</v>
+      </c>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="39"/>
-      <c r="B34" s="41" t="s">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="21"/>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18">
+        <v>5</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="33">
+        <f t="shared" ref="G35" si="2">PRODUCT(C35:F35)</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="23">
+        <v>500</v>
+      </c>
+      <c r="J35" s="33">
+        <f>G35*I35</f>
+        <v>500</v>
+      </c>
+      <c r="K35" s="21"/>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="39"/>
+      <c r="B37" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="42"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40">
-        <f>SUM(J9:J32)</f>
-        <v>518004.34040666668</v>
-      </c>
-      <c r="K34" s="35"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="53"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="52"/>
-    </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
-      <c r="B36" s="28" t="s">
+      <c r="C37" s="42"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40">
+        <f>SUM(J9:J35)</f>
+        <v>568854.64608666673</v>
+      </c>
+      <c r="K37" s="35"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="53"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="52"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="45"/>
+      <c r="B39" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="67">
-        <f>J34</f>
-        <v>518004.34040666668</v>
-      </c>
-      <c r="D36" s="67"/>
-      <c r="E36" s="38">
+      <c r="C39" s="61">
+        <f>J37</f>
+        <v>568854.64608666673</v>
+      </c>
+      <c r="D39" s="61"/>
+      <c r="E39" s="38">
         <v>100</v>
       </c>
-      <c r="F36" s="46"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="50"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="51"/>
-      <c r="B37" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="70">
-        <v>500000</v>
-      </c>
-      <c r="D37" s="70"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="44"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="51"/>
-      <c r="B38" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="70">
-        <f>C37-C40-C41</f>
-        <v>475000</v>
-      </c>
-      <c r="D38" s="70"/>
-      <c r="E38" s="38">
-        <f>C38/C36*100</f>
-        <v>91.698073345697168</v>
-      </c>
-      <c r="F38" s="44"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="44"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="51"/>
-      <c r="B39" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="67">
-        <f>C36-C38</f>
-        <v>43004.340406666684</v>
-      </c>
-      <c r="D39" s="67"/>
-      <c r="E39" s="38">
-        <f>100-E38</f>
-        <v>8.3019266543028323</v>
-      </c>
-      <c r="F39" s="44"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="44"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="50"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="51"/>
       <c r="B40" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="67">
-        <f>C37*0.03</f>
-        <v>15000</v>
-      </c>
-      <c r="D40" s="67"/>
-      <c r="E40" s="38">
-        <v>3</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C40" s="64">
+        <v>500000</v>
+      </c>
+      <c r="D40" s="64"/>
+      <c r="E40" s="38"/>
       <c r="F40" s="44"/>
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>
@@ -3670,15 +3680,16 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="51"/>
       <c r="B41" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="67">
-        <f>C37*0.02</f>
-        <v>10000</v>
-      </c>
-      <c r="D41" s="67"/>
+        <v>33</v>
+      </c>
+      <c r="C41" s="64">
+        <f>C40-C43-C44</f>
+        <v>475000</v>
+      </c>
+      <c r="D41" s="64"/>
       <c r="E41" s="38">
-        <v>2</v>
+        <f>C41/C39*100</f>
+        <v>83.501119884961312</v>
       </c>
       <c r="F41" s="44"/>
       <c r="G41" s="43"/>
@@ -3687,22 +3698,80 @@
       <c r="J41" s="43"/>
       <c r="K41" s="44"/>
     </row>
-    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="52"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
-    </row>
-    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="51"/>
+      <c r="B42" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="61">
+        <f>C39-C41</f>
+        <v>93854.646086666733</v>
+      </c>
+      <c r="D42" s="61"/>
+      <c r="E42" s="38">
+        <f>100-E41</f>
+        <v>16.498880115038688</v>
+      </c>
+      <c r="F42" s="44"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="44"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="51"/>
+      <c r="B43" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="61">
+        <f>C40*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D43" s="61"/>
+      <c r="E43" s="38">
+        <v>3</v>
+      </c>
+      <c r="F43" s="44"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="44"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="51"/>
+      <c r="B44" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="61">
+        <f>C40*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D44" s="61"/>
+      <c r="E44" s="38">
+        <v>2</v>
+      </c>
+      <c r="F44" s="44"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="44"/>
+    </row>
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="52"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="52"/>
+    </row>
     <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -3756,8 +3825,19 @@
     <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -3765,14 +3845,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -3783,7 +3855,7 @@
 </oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="24" max="10" man="1"/>
+    <brk id="26" max="10" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ganapati valuation given to upabhokta
</commit_message>
<xml_diff>
--- a/ofc/estimates/ganapati baatika mandir samrakxan/valuation ganapati batika pahiro samrakxan.xlsx
+++ b/ofc/estimates/ganapati baatika mandir samrakxan/valuation ganapati batika pahiro samrakxan.xlsx
@@ -2,30 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\ganapati baatika mandir samrakxan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\081-082\ofc\ofc\estimates\ganapati baatika mandir samrakxan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="re-estimate" sheetId="18" r:id="rId1"/>
     <sheet name="WCR" sheetId="6" r:id="rId2"/>
     <sheet name="V" sheetId="19" r:id="rId3"/>
+    <sheet name="M" sheetId="20" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
+    <definedName name="description_124" localSheetId="3">#REF!</definedName>
     <definedName name="description_124" localSheetId="0">#REF!</definedName>
     <definedName name="description_124" localSheetId="2">#REF!</definedName>
     <definedName name="description_124">#REF!</definedName>
@@ -42,13 +44,16 @@
     <definedName name="description_759">[1]Abstract!$B$278</definedName>
     <definedName name="description_781">[6]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">M!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'re-estimate'!$A$1:$K$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">V!$A$1:$K$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">WCR!$A$1:$K$26</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">M!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'re-estimate'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="58">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -221,19 +226,34 @@
     <t>Project:- गणपती गणेश मन्दिर मनोहरा नदीबाट कटान संरक्षण गर्ने</t>
   </si>
   <si>
-    <t xml:space="preserve">Date:2082/01/06       </t>
-  </si>
-  <si>
     <t xml:space="preserve">F.Y:2081/2082             </t>
+  </si>
+  <si>
+    <t>Detail Valuated Sheet</t>
+  </si>
+  <si>
+    <t>Total Valuated</t>
+  </si>
+  <si>
+    <t>Detail Quantity Measurement Sheet</t>
+  </si>
+  <si>
+    <t>Date: 2082/02/20</t>
+  </si>
+  <si>
+    <t>Date:2082/02/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date:2082/02/20       </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -388,9 +408,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -398,7 +418,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,14 +438,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -434,7 +454,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -458,7 +478,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,7 +513,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,7 +528,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -524,7 +544,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -533,6 +553,30 @@
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -544,25 +588,25 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -577,23 +621,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1303,134 +1334,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="66" t="s">
+      <c r="H6" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1465,7 +1496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -1482,7 +1513,7 @@
       <c r="J9" s="40"/>
       <c r="K9" s="58"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
         <v>43</v>
@@ -1510,7 +1541,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="36" t="s">
         <v>39</v>
@@ -1535,7 +1566,7 @@
       </c>
       <c r="K11" s="58"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="36" t="s">
         <v>45</v>
@@ -1553,7 +1584,7 @@
       </c>
       <c r="K12" s="60"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="36"/>
       <c r="C13" s="19"/>
@@ -1566,7 +1597,7 @@
       <c r="J13" s="40"/>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -1583,7 +1614,7 @@
       <c r="J14" s="40"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="36" t="str">
         <f>B10</f>
@@ -1612,7 +1643,7 @@
       <c r="J15" s="40"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="36" t="s">
         <v>39</v>
@@ -1637,7 +1668,7 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="36"/>
       <c r="C17" s="19"/>
@@ -1650,7 +1681,7 @@
       <c r="J17" s="40"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -1667,7 +1698,7 @@
       <c r="J18" s="40"/>
       <c r="K18" s="60"/>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="36" t="s">
         <v>43</v>
@@ -1693,7 +1724,7 @@
       <c r="J19" s="39"/>
       <c r="K19" s="58"/>
     </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="36"/>
       <c r="C20" s="35">
@@ -1718,7 +1749,7 @@
       <c r="J20" s="39"/>
       <c r="K20" s="58"/>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="36"/>
       <c r="C21" s="35">
@@ -1743,7 +1774,7 @@
       <c r="J21" s="39"/>
       <c r="K21" s="58"/>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="36" t="s">
         <v>39</v>
@@ -1776,7 +1807,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="36" t="s">
         <v>45</v>
@@ -1794,7 +1825,7 @@
       </c>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="36"/>
       <c r="C24" s="19"/>
@@ -1807,7 +1838,7 @@
       <c r="J24" s="40"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>4</v>
       </c>
@@ -1824,7 +1855,7 @@
       <c r="J25" s="40"/>
       <c r="K25" s="58"/>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="36" t="s">
         <v>47</v>
@@ -1849,7 +1880,7 @@
       <c r="J26" s="39"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="36" t="s">
         <v>39</v>
@@ -1882,7 +1913,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="36" t="s">
         <v>45</v>
@@ -1900,7 +1931,7 @@
       </c>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="36"/>
       <c r="C29" s="19"/>
@@ -1913,7 +1944,7 @@
       <c r="J29" s="40"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>5</v>
       </c>
@@ -1942,7 +1973,7 @@
       </c>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="24"/>
       <c r="C31" s="19"/>
@@ -1955,7 +1986,7 @@
       <c r="J31" s="40"/>
       <c r="K31" s="21"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="39"/>
       <c r="B32" s="41" t="s">
         <v>17</v>
@@ -1973,7 +2004,7 @@
       </c>
       <c r="K32" s="35"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="53"/>
       <c r="B33" s="56"/>
       <c r="C33" s="57"/>
@@ -1986,16 +2017,16 @@
       <c r="J33" s="55"/>
       <c r="K33" s="52"/>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="45"/>
       <c r="B34" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="61">
+      <c r="C34" s="69">
         <f>J32</f>
         <v>568746.79695333343</v>
       </c>
-      <c r="D34" s="61"/>
+      <c r="D34" s="69"/>
       <c r="E34" s="38">
         <v>100</v>
       </c>
@@ -2006,15 +2037,15 @@
       <c r="J34" s="49"/>
       <c r="K34" s="50"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="51"/>
       <c r="B35" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="64">
+      <c r="C35" s="72">
         <v>500000</v>
       </c>
-      <c r="D35" s="64"/>
+      <c r="D35" s="72"/>
       <c r="E35" s="38"/>
       <c r="F35" s="44"/>
       <c r="G35" s="43"/>
@@ -2023,16 +2054,16 @@
       <c r="J35" s="43"/>
       <c r="K35" s="44"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="51"/>
       <c r="B36" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="64">
+      <c r="C36" s="72">
         <f>C35-C38-C39</f>
         <v>475000</v>
       </c>
-      <c r="D36" s="64"/>
+      <c r="D36" s="72"/>
       <c r="E36" s="38">
         <f>C36/C34*100</f>
         <v>83.516953861451725</v>
@@ -2044,16 +2075,16 @@
       <c r="J36" s="43"/>
       <c r="K36" s="44"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="51"/>
       <c r="B37" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="61">
+      <c r="C37" s="69">
         <f>C34-C36</f>
         <v>93746.796953333425</v>
       </c>
-      <c r="D37" s="61"/>
+      <c r="D37" s="69"/>
       <c r="E37" s="38">
         <f>100-E36</f>
         <v>16.483046138548275</v>
@@ -2065,16 +2096,16 @@
       <c r="J37" s="43"/>
       <c r="K37" s="44"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="51"/>
       <c r="B38" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="61">
+      <c r="C38" s="69">
         <f>C35*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D38" s="61"/>
+      <c r="D38" s="69"/>
       <c r="E38" s="38">
         <v>3</v>
       </c>
@@ -2085,16 +2116,16 @@
       <c r="J38" s="43"/>
       <c r="K38" s="44"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="51"/>
       <c r="B39" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="61">
+      <c r="C39" s="69">
         <f>C35*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D39" s="61"/>
+      <c r="D39" s="69"/>
       <c r="E39" s="38">
         <v>2</v>
       </c>
@@ -2105,7 +2136,7 @@
       <c r="J39" s="43"/>
       <c r="K39" s="44"/>
     </row>
-    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="52"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
@@ -2118,71 +2149,64 @@
       <c r="J40" s="52"/>
       <c r="K40" s="52"/>
     </row>
-    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="A7:F7"/>
@@ -2191,6 +2215,13 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2208,112 +2239,112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+    </row>
+    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="75" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="71">
+      <c r="C6" s="79">
         <f>F26</f>
         <v>568746.79695333343</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2321,90 +2352,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="71">
+      <c r="J6" s="79">
         <f>I26</f>
-        <v>568854.64608666673</v>
-      </c>
-      <c r="K6" s="72"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>568795.26818666677</v>
+      </c>
+      <c r="K6" s="80"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="I7" s="79" t="s">
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="I7" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="65" t="str">
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="63" t="str">
         <f>'re-estimate'!A6:F6</f>
         <v>Project:- गणपती गणेश मन्दिर मनोहरा नदीबाट कटान संरक्षण गर्ने</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="I8" s="80" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="65" t="str">
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="I8" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="63" t="str">
         <f>'re-estimate'!A7:F7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="I9" s="80" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="76" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="I9" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="81" t="s">
+      <c r="D11" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81" t="s">
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="76" t="s">
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="77" t="s">
+      <c r="K11" s="74" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="76"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="73"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2423,10 +2454,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="76"/>
-      <c r="K12" s="77"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="J12" s="73"/>
+      <c r="K12" s="74"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <f>'re-estimate'!A9</f>
         <v>1</v>
@@ -2453,7 +2484,7 @@
       </c>
       <c r="G13" s="12">
         <f>V!G12</f>
-        <v>45.099999999999994</v>
+        <v>45.400000000000006</v>
       </c>
       <c r="H13" s="12">
         <f>V!I12</f>
@@ -2461,19 +2492,23 @@
       </c>
       <c r="I13" s="12">
         <f>G13*H13</f>
-        <v>2914.8129999999996</v>
+        <v>2934.2020000000002</v>
       </c>
       <c r="J13" s="27">
         <f>I13-F13</f>
-        <v>478.26199999999972</v>
+        <v>497.65100000000029</v>
       </c>
       <c r="K13" s="14"/>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M13" s="1">
+        <f>1.25*F13</f>
+        <v>3045.6887499999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
-      <c r="B14" s="32" t="str">
-        <f>'re-estimate'!B11</f>
-        <v>Sub-total</v>
+      <c r="B14" s="86" t="str">
+        <f>'re-estimate'!B12</f>
+        <v>-VAT 13% calculation</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2486,15 +2521,15 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12">
         <f>V!J13</f>
-        <v>314.06136666666663</v>
+        <v>316.15046666666672</v>
       </c>
       <c r="J14" s="27">
         <f>I14-F14</f>
-        <v>51.53113333333323</v>
+        <v>53.620233333333317</v>
       </c>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="12"/>
@@ -2507,7 +2542,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="26">
         <f>'re-estimate'!A14</f>
         <v>2</v>
@@ -2534,7 +2569,7 @@
       </c>
       <c r="G16" s="12">
         <f>V!G18</f>
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="H16" s="12">
         <f>V!I18</f>
@@ -2542,15 +2577,19 @@
       </c>
       <c r="I16" s="12">
         <f>G16*H16</f>
-        <v>2749.1039999999998</v>
+        <v>2668.2479999999996</v>
       </c>
       <c r="J16" s="27">
         <f>I16-F16</f>
-        <v>121.28400000000011</v>
+        <v>40.427999999999884</v>
       </c>
       <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="1">
+        <f>1.25*F16</f>
+        <v>3284.7749999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="12"/>
@@ -2563,7 +2602,7 @@
       <c r="J17" s="27"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="1" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A18" s="26">
         <f>'re-estimate'!A18</f>
         <v>3</v>
@@ -2606,9 +2645,9 @@
       </c>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
-      <c r="B19" s="32" t="str">
+      <c r="B19" s="86" t="str">
         <f>'re-estimate'!B23</f>
         <v>-VAT 13% calculation</v>
       </c>
@@ -2631,7 +2670,7 @@
       </c>
       <c r="K19" s="14"/>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="28"/>
       <c r="C20" s="12"/>
@@ -2644,7 +2683,7 @@
       <c r="J20" s="27"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A21" s="26">
         <f>'re-estimate'!A25</f>
         <v>4</v>
@@ -2687,9 +2726,9 @@
       </c>
       <c r="K21" s="14"/>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
-      <c r="B22" s="32" t="str">
+      <c r="B22" s="86" t="str">
         <f>'re-estimate'!B28</f>
         <v>-VAT 13% calculation</v>
       </c>
@@ -2712,7 +2751,7 @@
       </c>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="28"/>
       <c r="C23" s="12"/>
@@ -2725,7 +2764,7 @@
       <c r="J23" s="27"/>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26">
         <f>'re-estimate'!A30</f>
         <v>5</v>
@@ -2768,7 +2807,7 @@
       </c>
       <c r="K24" s="14"/>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="12"/>
@@ -2781,7 +2820,7 @@
       <c r="J25" s="27"/>
       <c r="K25" s="14"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6" t="s">
         <v>16</v>
@@ -2797,16 +2836,23 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7">
         <f>SUM(I13:I24)</f>
-        <v>568854.64608666673</v>
+        <v>568795.26818666677</v>
       </c>
       <c r="J26" s="13">
         <f>I26-F26</f>
-        <v>107.84913333330769</v>
+        <v>48.471233333344571</v>
       </c>
       <c r="K26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2820,13 +2866,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2844,134 +2883,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="66" t="s">
+      <c r="H6" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3006,7 +3045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -3023,7 +3062,7 @@
       <c r="J9" s="40"/>
       <c r="K9" s="58"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
         <v>43</v>
@@ -3032,26 +3071,25 @@
         <v>1</v>
       </c>
       <c r="D10" s="37">
-        <f>13</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="37">
-        <f>2.5+0.3+0.3</f>
-        <v>3.0999999999999996</v>
+        <f>2.5+0.2+0.2</f>
+        <v>2.9000000000000004</v>
       </c>
       <c r="F10" s="37">
         <v>1</v>
       </c>
       <c r="G10" s="38">
         <f>PRODUCT(C10:F10)</f>
-        <v>40.299999999999997</v>
+        <v>40.600000000000009</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="36"/>
       <c r="C11" s="35">
@@ -3076,7 +3114,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="58"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="36" t="s">
         <v>39</v>
@@ -3087,7 +3125,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="23">
         <f>SUM(G10:G11)</f>
-        <v>45.099999999999994</v>
+        <v>45.400000000000006</v>
       </c>
       <c r="H12" s="22" t="s">
         <v>38</v>
@@ -3097,11 +3135,11 @@
       </c>
       <c r="J12" s="40">
         <f>G12*I12</f>
-        <v>2914.8129999999996</v>
+        <v>2934.2020000000002</v>
       </c>
       <c r="K12" s="58"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="36" t="s">
         <v>45</v>
@@ -3115,11 +3153,11 @@
       <c r="I13" s="23"/>
       <c r="J13" s="40">
         <f>0.13*G12*19284/360</f>
-        <v>314.06136666666663</v>
+        <v>316.15046666666672</v>
       </c>
       <c r="K13" s="60"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="36"/>
       <c r="C14" s="19"/>
@@ -3132,7 +3170,7 @@
       <c r="J14" s="40"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -3149,7 +3187,7 @@
       <c r="J15" s="40"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="36" t="str">
         <f>B10</f>
@@ -3159,25 +3197,24 @@
         <v>1</v>
       </c>
       <c r="D16" s="20">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" s="21">
-        <f>0.5</f>
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="F16" s="21">
         <v>1</v>
       </c>
       <c r="G16" s="38">
         <f>PRODUCT(C16:F16)</f>
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="23"/>
       <c r="J16" s="40"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="36"/>
       <c r="C17" s="19">
@@ -3201,7 +3238,7 @@
       <c r="J17" s="40"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="36" t="s">
         <v>39</v>
@@ -3212,7 +3249,7 @@
       <c r="F18" s="21"/>
       <c r="G18" s="23">
         <f>SUM(G16:G17)</f>
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>38</v>
@@ -3222,11 +3259,11 @@
       </c>
       <c r="J18" s="40">
         <f>G18*I18</f>
-        <v>2749.1039999999998</v>
+        <v>2668.2479999999996</v>
       </c>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="36"/>
       <c r="C19" s="19"/>
@@ -3239,7 +3276,7 @@
       <c r="J19" s="40"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:14" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="225" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>3</v>
       </c>
@@ -3256,7 +3293,7 @@
       <c r="J20" s="40"/>
       <c r="K20" s="60"/>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="36" t="s">
         <v>43</v>
@@ -3282,7 +3319,7 @@
       <c r="J21" s="39"/>
       <c r="K21" s="58"/>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="36"/>
       <c r="C22" s="35">
@@ -3307,7 +3344,7 @@
       <c r="J22" s="39"/>
       <c r="K22" s="58"/>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="36"/>
       <c r="C23" s="35">
@@ -3332,7 +3369,7 @@
       <c r="J23" s="39"/>
       <c r="K23" s="58"/>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="36" t="s">
         <v>39</v>
@@ -3365,7 +3402,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="36" t="s">
         <v>45</v>
@@ -3383,7 +3420,7 @@
       </c>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="36"/>
       <c r="C26" s="19"/>
@@ -3396,7 +3433,7 @@
       <c r="J26" s="40"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>4</v>
       </c>
@@ -3413,7 +3450,7 @@
       <c r="J27" s="40"/>
       <c r="K27" s="58"/>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="36" t="s">
         <v>47</v>
@@ -3437,7 +3474,7 @@
       <c r="J28" s="39"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="36"/>
       <c r="C29" s="35">
@@ -3459,7 +3496,7 @@
       <c r="J29" s="39"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="36"/>
       <c r="C30" s="35">
@@ -3481,7 +3518,7 @@
       <c r="J30" s="39"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="36"/>
       <c r="C31" s="35">
@@ -3503,7 +3540,7 @@
       <c r="J31" s="39"/>
       <c r="K31" s="21"/>
     </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="36" t="s">
         <v>39</v>
@@ -3536,7 +3573,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="36" t="s">
         <v>45</v>
@@ -3554,7 +3591,7 @@
       </c>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="36"/>
       <c r="C34" s="19"/>
@@ -3567,7 +3604,7 @@
       <c r="J34" s="40"/>
       <c r="K34" s="21"/>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18">
         <v>5</v>
       </c>
@@ -3596,7 +3633,7 @@
       </c>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="24"/>
       <c r="C36" s="19"/>
@@ -3609,7 +3646,7 @@
       <c r="J36" s="40"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="39"/>
       <c r="B37" s="41" t="s">
         <v>17</v>
@@ -3623,11 +3660,11 @@
       <c r="I37" s="40"/>
       <c r="J37" s="40">
         <f>SUM(J9:J35)</f>
-        <v>568854.64608666673</v>
+        <v>568795.26818666677</v>
       </c>
       <c r="K37" s="35"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="53"/>
       <c r="B38" s="56"/>
       <c r="C38" s="57"/>
@@ -3640,16 +3677,16 @@
       <c r="J38" s="55"/>
       <c r="K38" s="52"/>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="45"/>
       <c r="B39" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="61">
+        <v>53</v>
+      </c>
+      <c r="C39" s="69">
         <f>J37</f>
-        <v>568854.64608666673</v>
-      </c>
-      <c r="D39" s="61"/>
+        <v>568795.26818666677</v>
+      </c>
+      <c r="D39" s="69"/>
       <c r="E39" s="38">
         <v>100</v>
       </c>
@@ -3660,15 +3697,15 @@
       <c r="J39" s="49"/>
       <c r="K39" s="50"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="51"/>
       <c r="B40" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="64">
+      <c r="C40" s="72">
         <v>500000</v>
       </c>
-      <c r="D40" s="64"/>
+      <c r="D40" s="72"/>
       <c r="E40" s="38"/>
       <c r="F40" s="44"/>
       <c r="G40" s="43"/>
@@ -3677,19 +3714,19 @@
       <c r="J40" s="43"/>
       <c r="K40" s="44"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
       <c r="B41" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="64">
+      <c r="C41" s="72">
         <f>C40-C43-C44</f>
         <v>475000</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="72"/>
       <c r="E41" s="38">
         <f>C41/C39*100</f>
-        <v>83.501119884961312</v>
+        <v>83.509836766805677</v>
       </c>
       <c r="F41" s="44"/>
       <c r="G41" s="43"/>
@@ -3698,19 +3735,19 @@
       <c r="J41" s="43"/>
       <c r="K41" s="44"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="51"/>
       <c r="B42" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="61">
+      <c r="C42" s="69">
         <f>C39-C41</f>
-        <v>93854.646086666733</v>
-      </c>
-      <c r="D42" s="61"/>
+        <v>93795.26818666677</v>
+      </c>
+      <c r="D42" s="69"/>
       <c r="E42" s="38">
         <f>100-E41</f>
-        <v>16.498880115038688</v>
+        <v>16.490163233194323</v>
       </c>
       <c r="F42" s="44"/>
       <c r="G42" s="43"/>
@@ -3719,16 +3756,16 @@
       <c r="J42" s="43"/>
       <c r="K42" s="44"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="51"/>
       <c r="B43" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="61">
+      <c r="C43" s="69">
         <f>C40*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D43" s="61"/>
+      <c r="D43" s="69"/>
       <c r="E43" s="38">
         <v>3</v>
       </c>
@@ -3739,16 +3776,16 @@
       <c r="J43" s="43"/>
       <c r="K43" s="44"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="51"/>
       <c r="B44" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="61">
+      <c r="C44" s="69">
         <f>C40*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D44" s="61"/>
+      <c r="D44" s="69"/>
       <c r="E44" s="38">
         <v>2</v>
       </c>
@@ -3759,7 +3796,7 @@
       <c r="J44" s="43"/>
       <c r="K44" s="44"/>
     </row>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="52"/>
       <c r="B45" s="52"/>
       <c r="C45" s="52"/>
@@ -3772,64 +3809,71 @@
       <c r="J45" s="52"/>
       <c r="K45" s="52"/>
     </row>
-    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="A7:F7"/>
@@ -3838,13 +3882,1020 @@
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="26" max="10" man="1"/>
+  </rowBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="3"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>1</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="35">
+        <v>1</v>
+      </c>
+      <c r="D10" s="37">
+        <v>14</v>
+      </c>
+      <c r="E10" s="37">
+        <f>2.5+0.2+0.2</f>
+        <v>2.9000000000000004</v>
+      </c>
+      <c r="F10" s="37">
+        <v>1</v>
+      </c>
+      <c r="G10" s="38">
+        <f>PRODUCT(C10:F10)</f>
+        <v>40.600000000000009</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="58"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="35">
+        <v>1</v>
+      </c>
+      <c r="D11" s="37">
+        <v>2</v>
+      </c>
+      <c r="E11" s="37">
+        <f>2+0.2+0.2</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="F11" s="37">
+        <v>1</v>
+      </c>
+      <c r="G11" s="38">
+        <f>PRODUCT(C11:F11)</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="23">
+        <f>SUM(G10:G11)</f>
+        <v>45.400000000000006</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="23">
+        <v>64.63</v>
+      </c>
+      <c r="J12" s="40">
+        <f>G12*I12</f>
+        <v>2934.2020000000002</v>
+      </c>
+      <c r="K12" s="58"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="40">
+        <f>0.13*G12*19284/360</f>
+        <v>316.15046666666672</v>
+      </c>
+      <c r="K13" s="60"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="36" t="str">
+        <f>B10</f>
+        <v>-for gabion wall</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20">
+        <v>14</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0.45</v>
+      </c>
+      <c r="F16" s="21">
+        <v>1</v>
+      </c>
+      <c r="G16" s="38">
+        <f>PRODUCT(C16:F16)</f>
+        <v>6.3</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="21"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="20">
+        <v>2</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="38">
+        <f>PRODUCT(C17:F17)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="23">
+        <f>SUM(G16:G17)</f>
+        <v>6.6</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="23">
+        <v>404.28</v>
+      </c>
+      <c r="J18" s="40">
+        <f>G18*I18</f>
+        <v>2668.2479999999996</v>
+      </c>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>3</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="60"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="35">
+        <v>1</v>
+      </c>
+      <c r="D21" s="37">
+        <v>3</v>
+      </c>
+      <c r="E21" s="37">
+        <v>1</v>
+      </c>
+      <c r="F21" s="37">
+        <v>1</v>
+      </c>
+      <c r="G21" s="38">
+        <f>PRODUCT(C21:F21)</f>
+        <v>3</v>
+      </c>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="58"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="35">
+        <f>(4+2+2)+8+3+2</f>
+        <v>21</v>
+      </c>
+      <c r="D22" s="37">
+        <v>2</v>
+      </c>
+      <c r="E22" s="37">
+        <v>1</v>
+      </c>
+      <c r="F22" s="37">
+        <v>1</v>
+      </c>
+      <c r="G22" s="38">
+        <f t="shared" ref="G22:G23" si="0">PRODUCT(C22:F22)</f>
+        <v>42</v>
+      </c>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="58"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="35">
+        <f>(8+4)+(2+4)+2+2</f>
+        <v>22</v>
+      </c>
+      <c r="D23" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="E23" s="37">
+        <v>1</v>
+      </c>
+      <c r="F23" s="37">
+        <v>1</v>
+      </c>
+      <c r="G23" s="38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="58"/>
+    </row>
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="23">
+        <f>SUM(G21:G23)</f>
+        <v>78</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="23">
+        <v>6509.3</v>
+      </c>
+      <c r="J24" s="40">
+        <f>G24*I24</f>
+        <v>507725.4</v>
+      </c>
+      <c r="K24" s="21"/>
+      <c r="M24">
+        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
+        <v>7485.69</v>
+      </c>
+      <c r="N24">
+        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
+        <v>4746.7977499999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="40">
+        <f>0.13*G24*4746.798</f>
+        <v>48132.531719999999</v>
+      </c>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>4</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="58"/>
+    </row>
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="35">
+        <v>1</v>
+      </c>
+      <c r="D28" s="37">
+        <v>14</v>
+      </c>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37">
+        <v>1</v>
+      </c>
+      <c r="G28" s="38">
+        <f>PRODUCT(C28:F28)</f>
+        <v>14</v>
+      </c>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="35">
+        <v>1</v>
+      </c>
+      <c r="D29" s="37">
+        <v>12</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37">
+        <v>1</v>
+      </c>
+      <c r="G29" s="38">
+        <f t="shared" ref="G29:G31" si="1">PRODUCT(C29:F29)</f>
+        <v>12</v>
+      </c>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="35">
+        <v>1</v>
+      </c>
+      <c r="D30" s="37">
+        <v>6</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37">
+        <v>1</v>
+      </c>
+      <c r="G30" s="38">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="21"/>
+    </row>
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="35">
+        <v>1</v>
+      </c>
+      <c r="D31" s="37">
+        <v>2</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37">
+        <v>2</v>
+      </c>
+      <c r="G31" s="38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="23">
+        <f>SUM(G28:G31)</f>
+        <v>36</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="23">
+        <v>161.41999999999999</v>
+      </c>
+      <c r="J32" s="40">
+        <f>G32*I32</f>
+        <v>5811.12</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="M32">
+        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
+        <v>7485.69</v>
+      </c>
+      <c r="N32">
+        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
+        <v>4746.7977499999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="40">
+        <f>0.13*G32*45360/300</f>
+        <v>707.61599999999999</v>
+      </c>
+      <c r="K33" s="21"/>
+    </row>
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="21"/>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>5</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="33">
+        <f t="shared" ref="G35" si="2">PRODUCT(C35:F35)</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="23">
+        <v>500</v>
+      </c>
+      <c r="J35" s="33">
+        <f>G35*I35</f>
+        <v>500</v>
+      </c>
+      <c r="K35" s="21"/>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="39"/>
+      <c r="B37" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40">
+        <f>SUM(J9:J35)</f>
+        <v>568795.26818666677</v>
+      </c>
+      <c r="K37" s="35"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="53"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="52"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="45"/>
+      <c r="B39" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="69">
+        <f>J37</f>
+        <v>568795.26818666677</v>
+      </c>
+      <c r="D39" s="69"/>
+      <c r="E39" s="38">
+        <v>100</v>
+      </c>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="50"/>
+    </row>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="51"/>
+      <c r="B40" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="72">
+        <v>500000</v>
+      </c>
+      <c r="D40" s="72"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="44"/>
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="51"/>
+      <c r="B41" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="72">
+        <f>C40-C43-C44</f>
+        <v>475000</v>
+      </c>
+      <c r="D41" s="72"/>
+      <c r="E41" s="38">
+        <f>C41/C39*100</f>
+        <v>83.509836766805677</v>
+      </c>
+      <c r="F41" s="44"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="44"/>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="51"/>
+      <c r="B42" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="69">
+        <f>C39-C41</f>
+        <v>93795.26818666677</v>
+      </c>
+      <c r="D42" s="69"/>
+      <c r="E42" s="38">
+        <f>100-E41</f>
+        <v>16.490163233194323</v>
+      </c>
+      <c r="F42" s="44"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="44"/>
+    </row>
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="51"/>
+      <c r="B43" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="69">
+        <f>C40*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D43" s="69"/>
+      <c r="E43" s="38">
+        <v>3</v>
+      </c>
+      <c r="F43" s="44"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="44"/>
+    </row>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="51"/>
+      <c r="B44" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="69">
+        <f>C40*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D44" s="69"/>
+      <c r="E44" s="38">
+        <v>2</v>
+      </c>
+      <c r="F44" s="44"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="44"/>
+    </row>
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="52"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="52"/>
+    </row>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
edited lakilla mandir wood works
</commit_message>
<xml_diff>
--- a/ofc/estimates/ganapati baatika mandir samrakxan/valuation ganapati batika pahiro samrakxan.xlsx
+++ b/ofc/estimates/ganapati baatika mandir samrakxan/valuation ganapati batika pahiro samrakxan.xlsx
@@ -2,28 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\081-082\ofc\ofc\estimates\ganapati baatika mandir samrakxan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\ganapati baatika mandir samrakxan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="re-estimate" sheetId="18" r:id="rId1"/>
     <sheet name="WCR" sheetId="6" r:id="rId2"/>
     <sheet name="V" sheetId="19" r:id="rId3"/>
     <sheet name="M" sheetId="20" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="21" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
@@ -53,7 +54,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">V!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="65">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -245,15 +246,36 @@
   </si>
   <si>
     <t xml:space="preserve">Date:2082/02/20       </t>
+  </si>
+  <si>
+    <t>JCB</t>
+  </si>
+  <si>
+    <t>VAT</t>
+  </si>
+  <si>
+    <t>Geotextile</t>
+  </si>
+  <si>
+    <t>mesh wire</t>
+  </si>
+  <si>
+    <t>selvrged wire</t>
+  </si>
+  <si>
+    <t>binding wire</t>
+  </si>
+  <si>
+    <t>boulder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -408,9 +430,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -418,7 +440,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,14 +460,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,7 +476,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -478,7 +500,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,7 +535,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,7 +550,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,7 +566,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -559,73 +581,76 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1338,130 +1363,130 @@
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="71" t="s">
+      <c r="H7" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1496,7 +1521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -1513,7 +1538,7 @@
       <c r="J9" s="40"/>
       <c r="K9" s="58"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
         <v>43</v>
@@ -1541,7 +1566,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="36" t="s">
         <v>39</v>
@@ -1566,7 +1591,7 @@
       </c>
       <c r="K11" s="58"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="36" t="s">
         <v>45</v>
@@ -1584,7 +1609,7 @@
       </c>
       <c r="K12" s="60"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="36"/>
       <c r="C13" s="19"/>
@@ -1597,7 +1622,7 @@
       <c r="J13" s="40"/>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>2</v>
       </c>
@@ -1614,7 +1639,7 @@
       <c r="J14" s="40"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="36" t="str">
         <f>B10</f>
@@ -1643,7 +1668,7 @@
       <c r="J15" s="40"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="36" t="s">
         <v>39</v>
@@ -1668,7 +1693,7 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="36"/>
       <c r="C17" s="19"/>
@@ -1681,7 +1706,7 @@
       <c r="J17" s="40"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>3</v>
       </c>
@@ -1698,7 +1723,7 @@
       <c r="J18" s="40"/>
       <c r="K18" s="60"/>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="36" t="s">
         <v>43</v>
@@ -1724,7 +1749,7 @@
       <c r="J19" s="39"/>
       <c r="K19" s="58"/>
     </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="36"/>
       <c r="C20" s="35">
@@ -1749,7 +1774,7 @@
       <c r="J20" s="39"/>
       <c r="K20" s="58"/>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="36"/>
       <c r="C21" s="35">
@@ -1774,7 +1799,7 @@
       <c r="J21" s="39"/>
       <c r="K21" s="58"/>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="36" t="s">
         <v>39</v>
@@ -1807,7 +1832,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="36" t="s">
         <v>45</v>
@@ -1825,7 +1850,7 @@
       </c>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="36"/>
       <c r="C24" s="19"/>
@@ -1838,7 +1863,7 @@
       <c r="J24" s="40"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>4</v>
       </c>
@@ -1855,7 +1880,7 @@
       <c r="J25" s="40"/>
       <c r="K25" s="58"/>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="36" t="s">
         <v>47</v>
@@ -1880,7 +1905,7 @@
       <c r="J26" s="39"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="36" t="s">
         <v>39</v>
@@ -1913,7 +1938,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="36" t="s">
         <v>45</v>
@@ -1931,7 +1956,7 @@
       </c>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="36"/>
       <c r="C29" s="19"/>
@@ -1944,7 +1969,7 @@
       <c r="J29" s="40"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <v>5</v>
       </c>
@@ -1973,7 +1998,7 @@
       </c>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="24"/>
       <c r="C31" s="19"/>
@@ -1986,7 +2011,7 @@
       <c r="J31" s="40"/>
       <c r="K31" s="21"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="39"/>
       <c r="B32" s="41" t="s">
         <v>17</v>
@@ -2004,7 +2029,7 @@
       </c>
       <c r="K32" s="35"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="53"/>
       <c r="B33" s="56"/>
       <c r="C33" s="57"/>
@@ -2017,16 +2042,16 @@
       <c r="J33" s="55"/>
       <c r="K33" s="52"/>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="45"/>
       <c r="B34" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="69">
+      <c r="C34" s="66">
         <f>J32</f>
         <v>568746.79695333343</v>
       </c>
-      <c r="D34" s="69"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="38">
         <v>100</v>
       </c>
@@ -2037,15 +2062,15 @@
       <c r="J34" s="49"/>
       <c r="K34" s="50"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="51"/>
       <c r="B35" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="72">
+      <c r="C35" s="69">
         <v>500000</v>
       </c>
-      <c r="D35" s="72"/>
+      <c r="D35" s="69"/>
       <c r="E35" s="38"/>
       <c r="F35" s="44"/>
       <c r="G35" s="43"/>
@@ -2054,16 +2079,16 @@
       <c r="J35" s="43"/>
       <c r="K35" s="44"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="51"/>
       <c r="B36" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="72">
+      <c r="C36" s="69">
         <f>C35-C38-C39</f>
         <v>475000</v>
       </c>
-      <c r="D36" s="72"/>
+      <c r="D36" s="69"/>
       <c r="E36" s="38">
         <f>C36/C34*100</f>
         <v>83.516953861451725</v>
@@ -2075,16 +2100,16 @@
       <c r="J36" s="43"/>
       <c r="K36" s="44"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="51"/>
       <c r="B37" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="69">
+      <c r="C37" s="66">
         <f>C34-C36</f>
         <v>93746.796953333425</v>
       </c>
-      <c r="D37" s="69"/>
+      <c r="D37" s="66"/>
       <c r="E37" s="38">
         <f>100-E36</f>
         <v>16.483046138548275</v>
@@ -2096,16 +2121,16 @@
       <c r="J37" s="43"/>
       <c r="K37" s="44"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="51"/>
       <c r="B38" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="69">
+      <c r="C38" s="66">
         <f>C35*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D38" s="69"/>
+      <c r="D38" s="66"/>
       <c r="E38" s="38">
         <v>3</v>
       </c>
@@ -2116,16 +2141,16 @@
       <c r="J38" s="43"/>
       <c r="K38" s="44"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="51"/>
       <c r="B39" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="69">
+      <c r="C39" s="66">
         <f>C35*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D39" s="69"/>
+      <c r="D39" s="66"/>
       <c r="E39" s="38">
         <v>2</v>
       </c>
@@ -2136,7 +2161,7 @@
       <c r="J39" s="43"/>
       <c r="K39" s="44"/>
     </row>
-    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="52"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
@@ -2149,64 +2174,71 @@
       <c r="J40" s="52"/>
       <c r="K40" s="52"/>
     </row>
-    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="A7:F7"/>
@@ -2215,13 +2247,6 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2245,106 +2270,106 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-    </row>
-    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+    </row>
+    <row r="2" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-    </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="83" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-    </row>
-    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="79">
+      <c r="C6" s="76">
         <f>F26</f>
         <v>568746.79695333343</v>
       </c>
-      <c r="D6" s="80"/>
+      <c r="D6" s="77"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2352,90 +2377,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="79">
+      <c r="J6" s="76">
         <f>I26</f>
         <v>568795.26818666677</v>
       </c>
-      <c r="K6" s="80"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K6" s="77"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="I7" s="76" t="s">
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="I7" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="str">
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="70" t="str">
         <f>'re-estimate'!A6:F6</f>
         <v>Project:- गणपती गणेश मन्दिर मनोहरा नदीबाट कटान संरक्षण गर्ने</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="I8" s="77" t="s">
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="I8" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="str">
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="70" t="str">
         <f>'re-estimate'!A7:F7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="I9" s="77" t="s">
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="I9" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78" t="s">
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="73" t="s">
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="74" t="s">
+      <c r="K11" s="82" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="81"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2454,10 +2479,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="74"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
         <f>'re-estimate'!A9</f>
         <v>1</v>
@@ -2504,9 +2529,9 @@
         <v>3045.6887499999998</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
-      <c r="B14" s="86" t="str">
+      <c r="B14" s="65" t="str">
         <f>'re-estimate'!B12</f>
         <v>-VAT 13% calculation</v>
       </c>
@@ -2529,7 +2554,7 @@
       </c>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="12"/>
@@ -2542,7 +2567,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="1" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
         <f>'re-estimate'!A14</f>
         <v>2</v>
@@ -2589,7 +2614,7 @@
         <v>3284.7749999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="12"/>
@@ -2602,7 +2627,7 @@
       <c r="J17" s="27"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <f>'re-estimate'!A18</f>
         <v>3</v>
@@ -2645,9 +2670,9 @@
       </c>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="26"/>
-      <c r="B19" s="86" t="str">
+      <c r="B19" s="65" t="str">
         <f>'re-estimate'!B23</f>
         <v>-VAT 13% calculation</v>
       </c>
@@ -2670,7 +2695,7 @@
       </c>
       <c r="K19" s="14"/>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28"/>
       <c r="B20" s="28"/>
       <c r="C20" s="12"/>
@@ -2683,7 +2708,7 @@
       <c r="J20" s="27"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A21" s="26">
         <f>'re-estimate'!A25</f>
         <v>4</v>
@@ -2726,9 +2751,9 @@
       </c>
       <c r="K21" s="14"/>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="26"/>
-      <c r="B22" s="86" t="str">
+      <c r="B22" s="65" t="str">
         <f>'re-estimate'!B28</f>
         <v>-VAT 13% calculation</v>
       </c>
@@ -2751,7 +2776,7 @@
       </c>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28"/>
       <c r="B23" s="28"/>
       <c r="C23" s="12"/>
@@ -2764,7 +2789,7 @@
       <c r="J23" s="27"/>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26">
         <f>'re-estimate'!A30</f>
         <v>5</v>
@@ -2807,7 +2832,7 @@
       </c>
       <c r="K24" s="14"/>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="12"/>
@@ -2820,7 +2845,7 @@
       <c r="J25" s="27"/>
       <c r="K25" s="14"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6" t="s">
         <v>16</v>
@@ -2846,13 +2871,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2866,6 +2884,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2881,136 +2906,136 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="71" t="s">
+      <c r="H7" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3045,7 +3070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -3062,7 +3087,7 @@
       <c r="J9" s="40"/>
       <c r="K9" s="58"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="36" t="s">
         <v>43</v>
@@ -3089,7 +3114,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="36"/>
       <c r="C11" s="35">
@@ -3114,7 +3139,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="58"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="36" t="s">
         <v>39</v>
@@ -3139,7 +3164,7 @@
       </c>
       <c r="K12" s="58"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="36" t="s">
         <v>45</v>
@@ -3157,7 +3182,7 @@
       </c>
       <c r="K13" s="60"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="36"/>
       <c r="C14" s="19"/>
@@ -3170,7 +3195,7 @@
       <c r="J14" s="40"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -3187,7 +3212,7 @@
       <c r="J15" s="40"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="36" t="str">
         <f>B10</f>
@@ -3214,7 +3239,7 @@
       <c r="J16" s="40"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="36"/>
       <c r="C17" s="19">
@@ -3238,7 +3263,7 @@
       <c r="J17" s="40"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="36" t="s">
         <v>39</v>
@@ -3263,7 +3288,7 @@
       </c>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="36"/>
       <c r="C19" s="19"/>
@@ -3276,7 +3301,7 @@
       <c r="J19" s="40"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>3</v>
       </c>
@@ -3293,7 +3318,7 @@
       <c r="J20" s="40"/>
       <c r="K20" s="60"/>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="36" t="s">
         <v>43</v>
@@ -3319,7 +3344,7 @@
       <c r="J21" s="39"/>
       <c r="K21" s="58"/>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="36"/>
       <c r="C22" s="35">
@@ -3344,7 +3369,7 @@
       <c r="J22" s="39"/>
       <c r="K22" s="58"/>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="36"/>
       <c r="C23" s="35">
@@ -3369,7 +3394,7 @@
       <c r="J23" s="39"/>
       <c r="K23" s="58"/>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="36" t="s">
         <v>39</v>
@@ -3401,8 +3426,12 @@
         <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
         <v>4746.7977499999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <f>(26798.3/6+27258.9/6+28483.6/6+28588.1/6)/4*G24</f>
+        <v>361168.92499999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="36" t="s">
         <v>45</v>
@@ -3420,7 +3449,7 @@
       </c>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="36"/>
       <c r="C26" s="19"/>
@@ -3433,7 +3462,7 @@
       <c r="J26" s="40"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <v>4</v>
       </c>
@@ -3450,7 +3479,7 @@
       <c r="J27" s="40"/>
       <c r="K27" s="58"/>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="36" t="s">
         <v>47</v>
@@ -3474,7 +3503,7 @@
       <c r="J28" s="39"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="36"/>
       <c r="C29" s="35">
@@ -3496,7 +3525,7 @@
       <c r="J29" s="39"/>
       <c r="K29" s="21"/>
     </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="36"/>
       <c r="C30" s="35">
@@ -3518,7 +3547,7 @@
       <c r="J30" s="39"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="36"/>
       <c r="C31" s="35">
@@ -3540,7 +3569,7 @@
       <c r="J31" s="39"/>
       <c r="K31" s="21"/>
     </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="36" t="s">
         <v>39</v>
@@ -3573,7 +3602,7 @@
         <v>4746.7977499999997</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18"/>
       <c r="B33" s="36" t="s">
         <v>45</v>
@@ -3591,7 +3620,7 @@
       </c>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18"/>
       <c r="B34" s="36"/>
       <c r="C34" s="19"/>
@@ -3604,7 +3633,7 @@
       <c r="J34" s="40"/>
       <c r="K34" s="21"/>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18">
         <v>5</v>
       </c>
@@ -3633,7 +3662,7 @@
       </c>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="24"/>
       <c r="C36" s="19"/>
@@ -3646,7 +3675,7 @@
       <c r="J36" s="40"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="39"/>
       <c r="B37" s="41" t="s">
         <v>17</v>
@@ -3664,7 +3693,7 @@
       </c>
       <c r="K37" s="35"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="53"/>
       <c r="B38" s="56"/>
       <c r="C38" s="57"/>
@@ -3677,16 +3706,16 @@
       <c r="J38" s="55"/>
       <c r="K38" s="52"/>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="45"/>
       <c r="B39" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="69">
+      <c r="C39" s="66">
         <f>J37</f>
         <v>568795.26818666677</v>
       </c>
-      <c r="D39" s="69"/>
+      <c r="D39" s="66"/>
       <c r="E39" s="38">
         <v>100</v>
       </c>
@@ -3697,15 +3726,15 @@
       <c r="J39" s="49"/>
       <c r="K39" s="50"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="51"/>
       <c r="B40" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="72">
+      <c r="C40" s="69">
         <v>500000</v>
       </c>
-      <c r="D40" s="72"/>
+      <c r="D40" s="69"/>
       <c r="E40" s="38"/>
       <c r="F40" s="44"/>
       <c r="G40" s="43"/>
@@ -3714,16 +3743,16 @@
       <c r="J40" s="43"/>
       <c r="K40" s="44"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="51"/>
       <c r="B41" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="72">
+      <c r="C41" s="69">
         <f>C40-C43-C44</f>
         <v>475000</v>
       </c>
-      <c r="D41" s="72"/>
+      <c r="D41" s="69"/>
       <c r="E41" s="38">
         <f>C41/C39*100</f>
         <v>83.509836766805677</v>
@@ -3735,16 +3764,16 @@
       <c r="J41" s="43"/>
       <c r="K41" s="44"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="51"/>
       <c r="B42" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="69">
+      <c r="C42" s="66">
         <f>C39-C41</f>
         <v>93795.26818666677</v>
       </c>
-      <c r="D42" s="69"/>
+      <c r="D42" s="66"/>
       <c r="E42" s="38">
         <f>100-E41</f>
         <v>16.490163233194323</v>
@@ -3756,16 +3785,16 @@
       <c r="J42" s="43"/>
       <c r="K42" s="44"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="51"/>
       <c r="B43" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="69">
+      <c r="C43" s="66">
         <f>C40*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D43" s="69"/>
+      <c r="D43" s="66"/>
       <c r="E43" s="38">
         <v>3</v>
       </c>
@@ -3776,16 +3805,16 @@
       <c r="J43" s="43"/>
       <c r="K43" s="44"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="51"/>
       <c r="B44" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="69">
+      <c r="C44" s="66">
         <f>C40*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D44" s="69"/>
+      <c r="D44" s="66"/>
       <c r="E44" s="38">
         <v>2</v>
       </c>
@@ -3796,7 +3825,7 @@
       <c r="J44" s="43"/>
       <c r="K44" s="44"/>
     </row>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="52"/>
       <c r="B45" s="52"/>
       <c r="C45" s="52"/>
@@ -3809,66 +3838,1081 @@
       <c r="J45" s="52"/>
       <c r="K45" s="52"/>
     </row>
-    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="26" max="10" man="1"/>
+  </rowBreaks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N101"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="3"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>1</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="35">
+        <v>1</v>
+      </c>
+      <c r="D10" s="37">
+        <v>14</v>
+      </c>
+      <c r="E10" s="37">
+        <f>2.5+0.2+0.2</f>
+        <v>2.9000000000000004</v>
+      </c>
+      <c r="F10" s="37">
+        <v>1</v>
+      </c>
+      <c r="G10" s="38">
+        <f>PRODUCT(C10:F10)</f>
+        <v>40.600000000000009</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="58"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="35">
+        <v>1</v>
+      </c>
+      <c r="D11" s="37">
+        <v>2</v>
+      </c>
+      <c r="E11" s="37">
+        <f>2+0.2+0.2</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="F11" s="37">
+        <v>1</v>
+      </c>
+      <c r="G11" s="38">
+        <f>PRODUCT(C11:F11)</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="23">
+        <f>SUM(G10:G11)</f>
+        <v>45.400000000000006</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="23">
+        <v>64.63</v>
+      </c>
+      <c r="J12" s="40">
+        <f>G12*I12</f>
+        <v>2934.2020000000002</v>
+      </c>
+      <c r="K12" s="58"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="40">
+        <f>0.13*G12*19284/360</f>
+        <v>316.15046666666672</v>
+      </c>
+      <c r="K13" s="60"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="1:11" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18"/>
+      <c r="B16" s="36" t="str">
+        <f>B10</f>
+        <v>-for gabion wall</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="20">
+        <v>14</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0.45</v>
+      </c>
+      <c r="F16" s="21">
+        <v>1</v>
+      </c>
+      <c r="G16" s="38">
+        <f>PRODUCT(C16:F16)</f>
+        <v>6.3</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="21"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="20">
+        <v>2</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="38">
+        <f>PRODUCT(C17:F17)</f>
+        <v>0.3</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="23">
+        <f>SUM(G16:G17)</f>
+        <v>6.6</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="23">
+        <v>404.28</v>
+      </c>
+      <c r="J18" s="40">
+        <f>G18*I18</f>
+        <v>2668.2479999999996</v>
+      </c>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="1:14" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>3</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="60"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="35">
+        <v>1</v>
+      </c>
+      <c r="D21" s="37">
+        <v>3</v>
+      </c>
+      <c r="E21" s="37">
+        <v>1</v>
+      </c>
+      <c r="F21" s="37">
+        <v>1</v>
+      </c>
+      <c r="G21" s="38">
+        <f>PRODUCT(C21:F21)</f>
+        <v>3</v>
+      </c>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="58"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="35">
+        <f>(4+2+2)+8+3+2</f>
+        <v>21</v>
+      </c>
+      <c r="D22" s="37">
+        <v>2</v>
+      </c>
+      <c r="E22" s="37">
+        <v>1</v>
+      </c>
+      <c r="F22" s="37">
+        <v>1</v>
+      </c>
+      <c r="G22" s="38">
+        <f t="shared" ref="G22:G23" si="0">PRODUCT(C22:F22)</f>
+        <v>42</v>
+      </c>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="58"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="35">
+        <f>(8+4)+(2+4)+2+2</f>
+        <v>22</v>
+      </c>
+      <c r="D23" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="E23" s="37">
+        <v>1</v>
+      </c>
+      <c r="F23" s="37">
+        <v>1</v>
+      </c>
+      <c r="G23" s="38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="58"/>
+    </row>
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="23">
+        <f>SUM(G21:G23)</f>
+        <v>78</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="23">
+        <v>6509.3</v>
+      </c>
+      <c r="J24" s="40">
+        <f>G24*I24</f>
+        <v>507725.4</v>
+      </c>
+      <c r="K24" s="21"/>
+      <c r="M24">
+        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
+        <v>7485.69</v>
+      </c>
+      <c r="N24">
+        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
+        <v>4746.7977499999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="40">
+        <f>0.13*G24*4746.798</f>
+        <v>48132.531719999999</v>
+      </c>
+      <c r="K25" s="21"/>
+    </row>
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="21"/>
+    </row>
+    <row r="27" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
+        <v>4</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="58"/>
+    </row>
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="35">
+        <v>1</v>
+      </c>
+      <c r="D28" s="37">
+        <v>14</v>
+      </c>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37">
+        <v>1</v>
+      </c>
+      <c r="G28" s="38">
+        <f>PRODUCT(C28:F28)</f>
+        <v>14</v>
+      </c>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="21"/>
+    </row>
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="35">
+        <v>1</v>
+      </c>
+      <c r="D29" s="37">
+        <v>12</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37">
+        <v>1</v>
+      </c>
+      <c r="G29" s="38">
+        <f t="shared" ref="G29:G31" si="1">PRODUCT(C29:F29)</f>
+        <v>12</v>
+      </c>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="35">
+        <v>1</v>
+      </c>
+      <c r="D30" s="37">
+        <v>6</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37">
+        <v>1</v>
+      </c>
+      <c r="G30" s="38">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="21"/>
+    </row>
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="35">
+        <v>1</v>
+      </c>
+      <c r="D31" s="37">
+        <v>2</v>
+      </c>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37">
+        <v>2</v>
+      </c>
+      <c r="G31" s="38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="23">
+        <f>SUM(G28:G31)</f>
+        <v>36</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="23">
+        <v>161.41999999999999</v>
+      </c>
+      <c r="J32" s="40">
+        <f>G32*I32</f>
+        <v>5811.12</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="M32">
+        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
+        <v>7485.69</v>
+      </c>
+      <c r="N32">
+        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
+        <v>4746.7977499999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="40">
+        <f>0.13*G32*45360/300</f>
+        <v>707.61599999999999</v>
+      </c>
+      <c r="K33" s="21"/>
+    </row>
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="21"/>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18">
+        <v>5</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="33">
+        <f t="shared" ref="G35" si="2">PRODUCT(C35:F35)</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="23">
+        <v>500</v>
+      </c>
+      <c r="J35" s="33">
+        <f>G35*I35</f>
+        <v>500</v>
+      </c>
+      <c r="K35" s="21"/>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="39"/>
+      <c r="B37" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40">
+        <f>SUM(J9:J35)</f>
+        <v>568795.26818666677</v>
+      </c>
+      <c r="K37" s="35"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="53"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="52"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="45"/>
+      <c r="B39" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="66">
+        <f>J37</f>
+        <v>568795.26818666677</v>
+      </c>
+      <c r="D39" s="66"/>
+      <c r="E39" s="38">
+        <v>100</v>
+      </c>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="50"/>
+    </row>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="51"/>
+      <c r="B40" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="69">
+        <v>500000</v>
+      </c>
+      <c r="D40" s="69"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="44"/>
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="51"/>
+      <c r="B41" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="69">
+        <f>C40-C43-C44</f>
+        <v>475000</v>
+      </c>
+      <c r="D41" s="69"/>
+      <c r="E41" s="38">
+        <f>C41/C39*100</f>
+        <v>83.509836766805677</v>
+      </c>
+      <c r="F41" s="44"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="44"/>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="51"/>
+      <c r="B42" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="66">
+        <f>C39-C41</f>
+        <v>93795.26818666677</v>
+      </c>
+      <c r="D42" s="66"/>
+      <c r="E42" s="38">
+        <f>100-E41</f>
+        <v>16.490163233194323</v>
+      </c>
+      <c r="F42" s="44"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="44"/>
+    </row>
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="51"/>
+      <c r="B43" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="66">
+        <f>C40*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D43" s="66"/>
+      <c r="E43" s="38">
+        <v>3</v>
+      </c>
+      <c r="F43" s="44"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="44"/>
+    </row>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="51"/>
+      <c r="B44" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="66">
+        <f>C40*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D44" s="66"/>
+      <c r="E44" s="38">
+        <v>2</v>
+      </c>
+      <c r="F44" s="44"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="44"/>
+    </row>
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="52"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="52"/>
+    </row>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
@@ -3877,7 +4921,6 @@
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -3897,1016 +4940,145 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N101"/>
+  <dimension ref="F7:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="2"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="62" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="61" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="16" t="s">
+    <row r="7" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="87"/>
+    </row>
+    <row r="11" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F11" s="5"/>
+      <c r="G11" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>1</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="58"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="35">
-        <v>1</v>
-      </c>
-      <c r="D10" s="37">
-        <v>14</v>
-      </c>
-      <c r="E10" s="37">
-        <f>2.5+0.2+0.2</f>
-        <v>2.9000000000000004</v>
-      </c>
-      <c r="F10" s="37">
-        <v>1</v>
-      </c>
-      <c r="G10" s="38">
-        <f>PRODUCT(C10:F10)</f>
-        <v>40.600000000000009</v>
-      </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="58"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="35">
-        <v>1</v>
-      </c>
-      <c r="D11" s="37">
-        <v>2</v>
-      </c>
-      <c r="E11" s="37">
-        <f>2+0.2+0.2</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="F11" s="37">
-        <v>1</v>
-      </c>
-      <c r="G11" s="38">
-        <f>PRODUCT(C11:F11)</f>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="58"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="23">
-        <f>SUM(G10:G11)</f>
-        <v>45.400000000000006</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="23">
-        <v>64.63</v>
-      </c>
-      <c r="J12" s="40">
-        <f>G12*I12</f>
-        <v>2934.2020000000002</v>
-      </c>
-      <c r="K12" s="58"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="40">
-        <f>0.13*G12*19284/360</f>
-        <v>316.15046666666672</v>
-      </c>
-      <c r="K13" s="60"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
-        <v>2</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="36" t="str">
-        <f>B10</f>
-        <v>-for gabion wall</v>
-      </c>
-      <c r="C16" s="19">
-        <v>1</v>
-      </c>
-      <c r="D16" s="20">
-        <v>14</v>
-      </c>
-      <c r="E16" s="21">
-        <v>0.45</v>
-      </c>
-      <c r="F16" s="21">
-        <v>1</v>
-      </c>
-      <c r="G16" s="38">
-        <f>PRODUCT(C16:F16)</f>
-        <v>6.3</v>
-      </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="19">
-        <v>1</v>
-      </c>
-      <c r="D17" s="20">
-        <v>2</v>
-      </c>
-      <c r="E17" s="21">
-        <v>0.3</v>
-      </c>
-      <c r="F17" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="38">
-        <f>PRODUCT(C17:F17)</f>
-        <v>0.3</v>
-      </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="23">
-        <f>SUM(G16:G17)</f>
-        <v>6.6</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="23">
-        <v>404.28</v>
-      </c>
-      <c r="J18" s="40">
-        <f>G18*I18</f>
-        <v>2668.2479999999996</v>
-      </c>
-      <c r="K18" s="21"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="1:14" ht="225" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>3</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="60"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="35">
-        <v>1</v>
-      </c>
-      <c r="D21" s="37">
-        <v>3</v>
-      </c>
-      <c r="E21" s="37">
-        <v>1</v>
-      </c>
-      <c r="F21" s="37">
-        <v>1</v>
-      </c>
-      <c r="G21" s="38">
-        <f>PRODUCT(C21:F21)</f>
-        <v>3</v>
-      </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="58"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="35">
-        <f>(4+2+2)+8+3+2</f>
-        <v>21</v>
-      </c>
-      <c r="D22" s="37">
-        <v>2</v>
-      </c>
-      <c r="E22" s="37">
-        <v>1</v>
-      </c>
-      <c r="F22" s="37">
-        <v>1</v>
-      </c>
-      <c r="G22" s="38">
-        <f t="shared" ref="G22:G23" si="0">PRODUCT(C22:F22)</f>
-        <v>42</v>
-      </c>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="58"/>
-    </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="35">
-        <f>(8+4)+(2+4)+2+2</f>
-        <v>22</v>
-      </c>
-      <c r="D23" s="37">
-        <v>1.5</v>
-      </c>
-      <c r="E23" s="37">
-        <v>1</v>
-      </c>
-      <c r="F23" s="37">
-        <v>1</v>
-      </c>
-      <c r="G23" s="38">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="58"/>
-    </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="23">
-        <f>SUM(G21:G23)</f>
-        <v>78</v>
-      </c>
-      <c r="H24" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="23">
-        <v>6509.3</v>
-      </c>
-      <c r="J24" s="40">
-        <f>G24*I24</f>
-        <v>507725.4</v>
-      </c>
-      <c r="K24" s="21"/>
-      <c r="M24">
-        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
-        <v>7485.69</v>
-      </c>
-      <c r="N24">
-        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
-        <v>4746.7977499999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="40">
-        <f>0.13*G24*4746.798</f>
-        <v>48132.531719999999</v>
-      </c>
-      <c r="K25" s="21"/>
-    </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="21"/>
-    </row>
-    <row r="27" spans="1:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
-        <v>4</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="58"/>
-    </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="35">
-        <v>1</v>
-      </c>
-      <c r="D28" s="37">
-        <v>14</v>
-      </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37">
-        <v>1</v>
-      </c>
-      <c r="G28" s="38">
-        <f>PRODUCT(C28:F28)</f>
-        <v>14</v>
-      </c>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="21"/>
-    </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="35">
-        <v>1</v>
-      </c>
-      <c r="D29" s="37">
-        <v>12</v>
-      </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37">
-        <v>1</v>
-      </c>
-      <c r="G29" s="38">
-        <f t="shared" ref="G29:G31" si="1">PRODUCT(C29:F29)</f>
-        <v>12</v>
-      </c>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="21"/>
-    </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="35">
-        <v>1</v>
-      </c>
-      <c r="D30" s="37">
-        <v>6</v>
-      </c>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37">
-        <v>1</v>
-      </c>
-      <c r="G30" s="38">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="21"/>
-    </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="35">
-        <v>1</v>
-      </c>
-      <c r="D31" s="37">
-        <v>2</v>
-      </c>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37">
-        <v>2</v>
-      </c>
-      <c r="G31" s="38">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="21"/>
-    </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="23">
-        <f>SUM(G28:G31)</f>
-        <v>36</v>
-      </c>
-      <c r="H32" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I32" s="23">
-        <v>161.41999999999999</v>
-      </c>
-      <c r="J32" s="40">
-        <f>G32*I32</f>
-        <v>5811.12</v>
-      </c>
-      <c r="K32" s="21"/>
-      <c r="M32">
-        <f>(7208.94+7297.22+[5]Rate_Analysis!$U$3091+[5]Rate_Analysis!$U$3104)/4</f>
-        <v>7485.69</v>
-      </c>
-      <c r="N32">
-        <f>([5]Rate_Analysis!$K$3063/6+[5]Rate_Analysis!$K$3076/6++[5]Rate_Analysis!$K$3089/6+[5]Rate_Analysis!$K$3102/6)/4</f>
-        <v>4746.7977499999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="40">
-        <f>0.13*G32*45360/300</f>
+      <c r="H11" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="88" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F12" s="88" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="89">
+        <f>19284/360*V!G12</f>
+        <v>2431.9266666666672</v>
+      </c>
+      <c r="H12" s="89">
+        <f>0.13*G12</f>
+        <v>316.15046666666677</v>
+      </c>
+      <c r="I12" s="89">
+        <f>SUM(G12:H12)</f>
+        <v>2748.0771333333341</v>
+      </c>
+    </row>
+    <row r="13" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F13" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="89">
+        <f>45360/300*V!G32</f>
+        <v>5443.2</v>
+      </c>
+      <c r="H13" s="89">
+        <f>0.13*G13</f>
         <v>707.61599999999999</v>
       </c>
-      <c r="K33" s="21"/>
-    </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="21"/>
-    </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
-        <v>5</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="19">
-        <v>1</v>
-      </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="33">
-        <f t="shared" ref="G35" si="2">PRODUCT(C35:F35)</f>
-        <v>1</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" s="23">
-        <v>500</v>
-      </c>
-      <c r="J35" s="33">
-        <f>G35*I35</f>
-        <v>500</v>
-      </c>
-      <c r="K35" s="21"/>
-    </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="21"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
-      <c r="B37" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40">
-        <f>SUM(J9:J35)</f>
-        <v>568795.26818666677</v>
-      </c>
-      <c r="K37" s="35"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="52"/>
-    </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45"/>
-      <c r="B39" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="69">
-        <f>J37</f>
-        <v>568795.26818666677</v>
-      </c>
-      <c r="D39" s="69"/>
-      <c r="E39" s="38">
-        <v>100</v>
-      </c>
-      <c r="F39" s="46"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="50"/>
-    </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
-      <c r="B40" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="72">
-        <v>500000</v>
-      </c>
-      <c r="D40" s="72"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="44"/>
-    </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
-      <c r="B41" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="72">
-        <f>C40-C43-C44</f>
-        <v>475000</v>
-      </c>
-      <c r="D41" s="72"/>
-      <c r="E41" s="38">
-        <f>C41/C39*100</f>
-        <v>83.509836766805677</v>
-      </c>
-      <c r="F41" s="44"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="44"/>
-    </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
-      <c r="B42" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="69">
-        <f>C39-C41</f>
-        <v>93795.26818666677</v>
-      </c>
-      <c r="D42" s="69"/>
-      <c r="E42" s="38">
-        <f>100-E41</f>
-        <v>16.490163233194323</v>
-      </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="44"/>
-    </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
-      <c r="B43" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="69">
-        <f>C40*0.03</f>
-        <v>15000</v>
-      </c>
-      <c r="D43" s="69"/>
-      <c r="E43" s="38">
-        <v>3</v>
-      </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="44"/>
-    </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
-      <c r="B44" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="69">
-        <f>C40*0.02</f>
-        <v>10000</v>
-      </c>
-      <c r="D44" s="69"/>
-      <c r="E44" s="38">
-        <v>2</v>
-      </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="44"/>
-    </row>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="52"/>
-    </row>
-    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="I13" s="89">
+        <f>SUM(G13:H13)</f>
+        <v>6150.8159999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F14" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="89">
+        <f>((9055.8/6+9346.05/6+10191/6+10185.84/6)/4)*V!G24</f>
+        <v>126030.74250000001</v>
+      </c>
+      <c r="H14" s="89">
+        <f>0.13*G14</f>
+        <v>16383.996525000002</v>
+      </c>
+      <c r="I14" s="89">
+        <f>SUM(G14:H14)</f>
+        <v>142414.73902500002</v>
+      </c>
+    </row>
+    <row r="15" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F15" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="89">
+        <f>((1008.78/6+1145.52/6+1393.2/6+1555.74/6)/4)*V!G24</f>
+        <v>16585.53</v>
+      </c>
+      <c r="H15" s="89">
+        <f>0.13*G15</f>
+        <v>2156.1188999999999</v>
+      </c>
+      <c r="I15" s="89">
+        <f>SUM(G15:H15)</f>
+        <v>18741.6489</v>
+      </c>
+    </row>
+    <row r="16" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F16" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="89">
+        <f>((434.4/6+468/6+600/6+547.2/6)/4)*V!G24</f>
+        <v>6661.1999999999989</v>
+      </c>
+      <c r="H16" s="89">
+        <f>0.13*G16</f>
+        <v>865.9559999999999</v>
+      </c>
+      <c r="I16" s="89">
+        <f>SUM(G16:H16)</f>
+        <v>7527.155999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F17" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="89">
+        <f>((16997.904*4/6)/4)*V!G24</f>
+        <v>220972.75200000001</v>
+      </c>
+      <c r="H17" s="89">
+        <f>0.13*G17</f>
+        <v>28726.457760000001</v>
+      </c>
+      <c r="I17" s="89">
+        <f>SUM(G17:H17)</f>
+        <v>249699.20976</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter xml:space="preserve">&amp;LPrepared By:
-&amp;CChecked By:
-&amp;RApproved By:
-</oddFooter>
-  </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="26" max="10" man="1"/>
-  </rowBreaks>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>